<commit_message>
update files per accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INFONEXT000/INFONEXT_SRL/EVAC/V.3.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111INFONEXT000/INFONEXT_SRL/EVAC/V.3.0.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\infonext\it-fse-accreditamento\GATEWAY\A1#111INFONEXT000\INFONEXT_SRL\EVAC\V.3.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86174E5-48DF-41BA-8697-1F64077F13E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3114E8CB-AE0F-49A9-AD8D-C98DDF818C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15420" yWindow="0" windowWidth="13485" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -2113,76 +2113,76 @@
     <t>2023-02-26T11:34:54Z</t>
   </si>
   <si>
-    <t>ec00e03d9be849bb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.80eeee6bdce1984a44a8cf4c505b8f47ef6d4860701be034f1997c245de7529b.5c31be7271^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T19:10:40Z</t>
-  </si>
-  <si>
-    <t>9130c4a3656ca80a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.28cdcac6637939c6a8dbd0b47956b5aadaee00568c6e8247ab9089f043750d28.096961d1f5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T19:14:12Z</t>
-  </si>
-  <si>
-    <t>11751fe75a10e54b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.bbbb091976c7aede6f6931634a8d920b0b24a547b2364c484caf762880ec3322.ac8b712b57^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T19:16:27Z</t>
-  </si>
-  <si>
-    <t>7f575ba625515b38</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.3e5771e5c8d898c14c4c5b398680bd81ff093871113dab013d842810089330ab.4d86612ef8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T19:18:43Z</t>
-  </si>
-  <si>
-    <t>061b0fc78e0a9121</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.24c36b8d91ea7c44c06a8ec57c9201c456aae406676be448609777a2d9811400.7e9e09cc41^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T19:20:55Z</t>
-  </si>
-  <si>
-    <t>eac3892248ee95c2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.3448cadfe205e7d9352b2483e95de95e0fbd97ef8cf26561743329f5ae305080.bd507baf7f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T19:23:06Z</t>
-  </si>
-  <si>
-    <t>cc813a4a068316df</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5526fb95c16d7661f432a2468d508e9a7d20e8199152e4de34af44e2cad1cdca.69ccc6b26c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T19:26:47Z</t>
-  </si>
-  <si>
-    <t>79780cb3c7d43314</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c3138ce54da4e77800438a8c07ae5d4fd5b14a2644d7810a6e3811ef6501e519.db312c1bd5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T19:28:55Z</t>
+    <t>2023-04-11T08:55:41Z</t>
+  </si>
+  <si>
+    <t>ba1dc1c2ba59def6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.80eeee6bdce1984a44a8cf4c505b8f47ef6d4860701be034f1997c245de7529b.3b2d65840c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T08:59:43Z</t>
+  </si>
+  <si>
+    <t>556d3903216a7d00</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.28cdcac6637939c6a8dbd0b47956b5aadaee00568c6e8247ab9089f043750d28.7eff601513^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T09:05:32Z</t>
+  </si>
+  <si>
+    <t>a1a41b1e64605e9f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.bbbb091976c7aede6f6931634a8d920b0b24a547b2364c484caf762880ec3322.cff7cfb527^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T09:10:33Z</t>
+  </si>
+  <si>
+    <t>60602dec82adc69d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.3e5771e5c8d898c14c4c5b398680bd81ff093871113dab013d842810089330ab.6735f8dc9a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T09:17:29Z</t>
+  </si>
+  <si>
+    <t>e869ae0536b82baa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.24c36b8d91ea7c44c06a8ec57c9201c456aae406676be448609777a2d9811400.28bed5c17b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T09:52:15Z</t>
+  </si>
+  <si>
+    <t>96f52fe87979184a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.3448cadfe205e7d9352b2483e95de95e0fbd97ef8cf26561743329f5ae305080.d585eb8079^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T09:54:56Z</t>
+  </si>
+  <si>
+    <t>b6a619e0bddfc41a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5526fb95c16d7661f432a2468d508e9a7d20e8199152e4de34af44e2cad1cdca.20c720e506^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T10:02:19Z</t>
+  </si>
+  <si>
+    <t>5b5878a8abbc8ec9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c3138ce54da4e77800438a8c07ae5d4fd5b14a2644d7810a6e3811ef6501e519.c0cf4fc354^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2677,7 +2677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2852,6 +2852,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4301,11 +4305,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B112" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E118" sqref="E118"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5024,17 +5028,17 @@
       <c r="E23" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="37">
-        <v>45004</v>
-      </c>
-      <c r="G23" s="36" t="s">
+      <c r="F23" s="59">
+        <v>45027</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="H23" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="I23" s="37" t="s">
         <v>411</v>
-      </c>
-      <c r="H23" s="36" t="s">
-        <v>409</v>
-      </c>
-      <c r="I23" s="36" t="s">
-        <v>410</v>
       </c>
       <c r="J23" s="39" t="s">
         <v>84</v>
@@ -5068,19 +5072,19 @@
       <c r="E24" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="37">
-        <v>45004</v>
-      </c>
-      <c r="G24" s="36" t="s">
+      <c r="F24" s="59">
+        <v>45027</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>412</v>
+      </c>
+      <c r="H24" s="37" t="s">
+        <v>413</v>
+      </c>
+      <c r="I24" s="37" t="s">
         <v>414</v>
       </c>
-      <c r="H24" s="36" t="s">
-        <v>412</v>
-      </c>
-      <c r="I24" s="36" t="s">
-        <v>413</v>
-      </c>
-      <c r="J24" s="39" t="s">
+      <c r="J24" s="37" t="s">
         <v>84</v>
       </c>
       <c r="K24" s="39"/>
@@ -5112,17 +5116,17 @@
       <c r="E25" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F25" s="37">
-        <v>45004</v>
-      </c>
-      <c r="G25" s="36" t="s">
+      <c r="F25" s="59">
+        <v>45027</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>415</v>
+      </c>
+      <c r="H25" s="37" t="s">
+        <v>416</v>
+      </c>
+      <c r="I25" s="37" t="s">
         <v>417</v>
-      </c>
-      <c r="H25" s="36" t="s">
-        <v>415</v>
-      </c>
-      <c r="I25" s="36" t="s">
-        <v>416</v>
       </c>
       <c r="J25" s="39" t="s">
         <v>84</v>
@@ -5156,17 +5160,17 @@
       <c r="E26" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="F26" s="37">
-        <v>45004</v>
-      </c>
-      <c r="G26" s="36" t="s">
+      <c r="F26" s="59">
+        <v>45027</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="H26" s="37" t="s">
+        <v>419</v>
+      </c>
+      <c r="I26" s="37" t="s">
         <v>420</v>
-      </c>
-      <c r="H26" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="I26" s="36" t="s">
-        <v>419</v>
       </c>
       <c r="J26" s="39" t="s">
         <v>84</v>
@@ -5200,17 +5204,17 @@
       <c r="E27" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="37">
-        <v>45004</v>
-      </c>
-      <c r="G27" s="36" t="s">
+      <c r="F27" s="59">
+        <v>45027</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>422</v>
+      </c>
+      <c r="I27" s="36" t="s">
         <v>423</v>
-      </c>
-      <c r="H27" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="I27" s="36" t="s">
-        <v>422</v>
       </c>
       <c r="J27" s="39" t="s">
         <v>84</v>
@@ -5244,17 +5248,17 @@
       <c r="E28" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="37">
-        <v>45004</v>
-      </c>
-      <c r="G28" s="36" t="s">
+      <c r="F28" s="59">
+        <v>45027</v>
+      </c>
+      <c r="G28" s="38" t="s">
+        <v>424</v>
+      </c>
+      <c r="H28" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="I28" s="37" t="s">
         <v>426</v>
-      </c>
-      <c r="H28" s="36" t="s">
-        <v>424</v>
-      </c>
-      <c r="I28" s="36" t="s">
-        <v>425</v>
       </c>
       <c r="J28" s="39" t="s">
         <v>84</v>
@@ -5288,17 +5292,17 @@
       <c r="E29" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="37">
-        <v>45004</v>
-      </c>
-      <c r="G29" s="36" t="s">
+      <c r="F29" s="59">
+        <v>45027</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>427</v>
+      </c>
+      <c r="H29" s="37" t="s">
+        <v>428</v>
+      </c>
+      <c r="I29" s="37" t="s">
         <v>429</v>
-      </c>
-      <c r="H29" s="36" t="s">
-        <v>427</v>
-      </c>
-      <c r="I29" s="36" t="s">
-        <v>428</v>
       </c>
       <c r="J29" s="39" t="s">
         <v>84</v>
@@ -5332,17 +5336,17 @@
       <c r="E30" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="37">
-        <v>45004</v>
-      </c>
-      <c r="G30" s="36" t="s">
+      <c r="F30" s="59">
+        <v>45027</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>430</v>
+      </c>
+      <c r="H30" s="37" t="s">
+        <v>431</v>
+      </c>
+      <c r="I30" s="37" t="s">
         <v>432</v>
-      </c>
-      <c r="H30" s="36" t="s">
-        <v>430</v>
-      </c>
-      <c r="I30" s="36" t="s">
-        <v>431</v>
       </c>
       <c r="J30" s="39" t="s">
         <v>84</v>
@@ -26340,6 +26344,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -26570,27 +26594,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26609,31 +26638,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>